<commit_message>
necessary alteration to 96 random word generation code
</commit_message>
<xml_diff>
--- a/DRM/sampled_random_words.xlsx
+++ b/DRM/sampled_random_words.xlsx
@@ -443,672 +443,672 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>hatred</t>
+          <t>mug</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>gloves</t>
+          <t>time</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>far</t>
+          <t>capital</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>england</t>
+          <t>rage</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>music</t>
+          <t>navy</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>smell</t>
+          <t>climb</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>fat</t>
+          <t>boat</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>vehicle</t>
+          <t>measuring</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>gin</t>
+          <t>ire</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>hospital</t>
+          <t>horn</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>new york</t>
+          <t>fury</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>stink</t>
+          <t>sandpaper</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>pile</t>
+          <t>honey</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>day</t>
+          <t>green</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>ivy</t>
+          <t>country</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>big</t>
+          <t>soft</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>country</t>
+          <t>united states</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>chess</t>
+          <t>uneven</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>coffee</t>
+          <t>swim</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>slow</t>
+          <t>slaw</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>waste</t>
+          <t>cautious</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>liquor</t>
+          <t>black</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>bumpy</t>
+          <t>palace</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>on</t>
+          <t>lungs</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>heart</t>
+          <t>chocolate</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>concert</t>
+          <t>legs</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>bulb</t>
+          <t>leg</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>dog</t>
+          <t>danger</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>physician</t>
+          <t>happiness</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>soft</t>
+          <t>road</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>tire</t>
+          <t>room</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>injection</t>
+          <t>desire</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>whiff</t>
+          <t>bad</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>tired</t>
+          <t>molehill</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>soda</t>
+          <t>clouds</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>danger</t>
+          <t>disease</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>lungs</t>
+          <t>melody</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>brook</t>
+          <t>water</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>beef</t>
+          <t>hand</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>butter</t>
+          <t>glass</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>bic</t>
+          <t>throne</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>hill</t>
+          <t>house</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>home</t>
+          <t>shout</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>slaw</t>
+          <t>pollution</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>grape</t>
+          <t>tobacco</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>sofa</t>
+          <t>gloves</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>lighter</t>
+          <t>eat</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>leg</t>
+          <t>picture</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>wing</t>
+          <t>dump</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>tune</t>
+          <t>dentist</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>shout</t>
+          <t>wood</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>fellow</t>
+          <t>flow</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>see</t>
+          <t>seat</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>goat</t>
+          <t>elastic</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>gulliver</t>
+          <t>snore</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>stream</t>
+          <t>keys</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>short</t>
+          <t>slice</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>goblet</t>
+          <t>see</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>bottles</t>
+          <t>stein</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>ugly</t>
+          <t>vines</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>bed</t>
+          <t>veal</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>dough</t>
+          <t>head</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>loud</t>
+          <t>sing</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>ill</t>
+          <t>lamb</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>scent</t>
+          <t>highway</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>stethoscope</t>
+          <t>quick</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>sharp</t>
+          <t>tune</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>awake</t>
+          <t>temper</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>inch</t>
+          <t>saucer</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>creek</t>
+          <t>emblem</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>billows</t>
+          <t>blow</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>garden</t>
+          <t>lake</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>lovely</t>
+          <t>halt</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>sorrow</t>
+          <t>anthem</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>mountain</t>
+          <t>fair</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>ring</t>
+          <t>goat</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>furnace</t>
+          <t>automobile</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>emblem</t>
+          <t>lawyer</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>scribble</t>
+          <t>scraps</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>touch</t>
+          <t>summer</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>patch</t>
+          <t>heat</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>sheep</t>
+          <t>peak</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>shooter</t>
+          <t>quill</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>office</t>
+          <t>leak</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>lettuce</t>
+          <t>cook</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>difficulty</t>
+          <t>fragrance</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>anthem</t>
+          <t>marker</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>want</t>
+          <t>crowded</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>air force</t>
+          <t>wake</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>bright</t>
+          <t>bike</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>people</t>
+          <t>swivel</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>noise</t>
+          <t>cushion</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>floor</t>
+          <t>beer</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>doctor</t>
+          <t>thin</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>sit</t>
+          <t>mad</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>dump</t>
+          <t>sour</t>
         </is>
       </c>
     </row>

</xml_diff>